<commit_message>
Validation: changed spreadsheet interval to 1 s to be consistent with other sprinkler simulations in the validation suite.
</commit_message>
<xml_diff>
--- a/cfast/trunk/Validation/UL_NFPRF/UL_NFPRF Sprinklers.xlsx
+++ b/cfast/trunk/Validation/UL_NFPRF/UL_NFPRF Sprinklers.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16065" yWindow="3720" windowWidth="25605" windowHeight="18375" tabRatio="500"/>
+    <workbookView xWindow="16065" yWindow="3720" windowWidth="25605" windowHeight="18375" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Parameters" sheetId="1" r:id="rId1"/>
     <sheet name="Sprinklers" sheetId="2" r:id="rId2"/>
     <sheet name="Burner Positions" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -573,7 +573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -1433,8 +1433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1533,478 +1533,478 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="B10" s="6">
-        <v>10.69</v>
+        <v>28.98</v>
       </c>
       <c r="C10" s="6">
-        <v>4.5199999999999996</v>
+        <v>13.66</v>
       </c>
       <c r="D10" s="6">
         <v>7.46</v>
       </c>
       <c r="F10">
         <f>B10-A$5</f>
-        <v>1.2899999999999991</v>
+        <v>19.579999999999998</v>
       </c>
       <c r="G10">
-        <f t="shared" ref="G10:H10" si="1">C10-B$5</f>
-        <v>0.51999999999999957</v>
+        <f>C10-B$5</f>
+        <v>9.66</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
+        <f>D10-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="B11" s="6">
-        <v>13.74</v>
+        <v>28.98</v>
       </c>
       <c r="C11" s="6">
-        <v>4.5199999999999996</v>
+        <v>16.71</v>
       </c>
       <c r="D11" s="6">
         <v>7.46</v>
       </c>
       <c r="F11">
-        <f t="shared" ref="F11:F58" si="2">B11-A$5</f>
-        <v>4.34</v>
+        <f>B11-A$5</f>
+        <v>19.579999999999998</v>
       </c>
       <c r="G11">
-        <f t="shared" ref="G11:G58" si="3">C11-B$5</f>
-        <v>0.51999999999999957</v>
+        <f>C11-B$5</f>
+        <v>12.71</v>
       </c>
       <c r="H11">
-        <f t="shared" ref="H11:H58" si="4">D11-C$5</f>
+        <f>D11-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="B12" s="6">
-        <v>16.79</v>
+        <v>28.98</v>
       </c>
       <c r="C12" s="6">
-        <v>4.5199999999999996</v>
+        <v>19.760000000000002</v>
       </c>
       <c r="D12" s="6">
         <v>7.46</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
-        <v>7.3899999999999988</v>
+        <f>B12-A$5</f>
+        <v>19.579999999999998</v>
       </c>
       <c r="G12">
-        <f t="shared" si="3"/>
-        <v>0.51999999999999957</v>
+        <f>C12-B$5</f>
+        <v>15.760000000000002</v>
       </c>
       <c r="H12">
-        <f t="shared" si="4"/>
+        <f>D12-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="B13" s="6">
-        <v>19.84</v>
+        <v>28.98</v>
       </c>
       <c r="C13" s="6">
-        <v>4.5199999999999996</v>
+        <v>22.81</v>
       </c>
       <c r="D13" s="6">
         <v>7.46</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
-        <v>10.44</v>
+        <f>B13-A$5</f>
+        <v>19.579999999999998</v>
       </c>
       <c r="G13">
-        <f t="shared" si="3"/>
-        <v>0.51999999999999957</v>
+        <f>C13-B$5</f>
+        <v>18.809999999999999</v>
       </c>
       <c r="H13">
-        <f t="shared" si="4"/>
+        <f>D13-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="B14" s="6">
-        <v>22.88</v>
+        <v>25.93</v>
       </c>
       <c r="C14" s="6">
-        <v>4.5199999999999996</v>
+        <v>13.66</v>
       </c>
       <c r="D14" s="6">
         <v>7.46</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
-        <v>13.479999999999999</v>
+        <f>B14-A$5</f>
+        <v>16.53</v>
       </c>
       <c r="G14">
-        <f t="shared" si="3"/>
-        <v>0.51999999999999957</v>
+        <f>C14-B$5</f>
+        <v>9.66</v>
       </c>
       <c r="H14">
-        <f t="shared" si="4"/>
+        <f>D14-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="B15" s="6">
         <v>25.93</v>
       </c>
       <c r="C15" s="6">
-        <v>4.5199999999999996</v>
+        <v>16.71</v>
       </c>
       <c r="D15" s="6">
         <v>7.46</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
+        <f>B15-A$5</f>
         <v>16.53</v>
       </c>
       <c r="G15">
-        <f t="shared" si="3"/>
-        <v>0.51999999999999957</v>
+        <f>C15-B$5</f>
+        <v>12.71</v>
       </c>
       <c r="H15">
-        <f t="shared" si="4"/>
+        <f>D15-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B16" s="6">
-        <v>28.98</v>
+        <v>25.93</v>
       </c>
       <c r="C16" s="6">
-        <v>4.5199999999999996</v>
+        <v>19.760000000000002</v>
       </c>
       <c r="D16" s="6">
         <v>7.46</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
-        <v>19.579999999999998</v>
+        <f>B16-A$5</f>
+        <v>16.53</v>
       </c>
       <c r="G16">
-        <f t="shared" si="3"/>
-        <v>0.51999999999999957</v>
+        <f>C16-B$5</f>
+        <v>15.760000000000002</v>
       </c>
       <c r="H16">
-        <f t="shared" si="4"/>
+        <f>D16-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="B17" s="6">
-        <v>10.69</v>
+        <v>25.93</v>
       </c>
       <c r="C17" s="6">
-        <v>7.57</v>
+        <v>22.81</v>
       </c>
       <c r="D17" s="6">
         <v>7.46</v>
       </c>
       <c r="F17">
-        <f t="shared" si="2"/>
-        <v>1.2899999999999991</v>
+        <f>B17-A$5</f>
+        <v>16.53</v>
       </c>
       <c r="G17">
-        <f t="shared" si="3"/>
-        <v>3.5700000000000003</v>
+        <f>C17-B$5</f>
+        <v>18.809999999999999</v>
       </c>
       <c r="H17">
-        <f t="shared" si="4"/>
+        <f>D17-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="B18" s="6">
-        <v>13.74</v>
+        <v>22.88</v>
       </c>
       <c r="C18" s="6">
-        <v>7.57</v>
+        <v>13.66</v>
       </c>
       <c r="D18" s="6">
         <v>7.46</v>
       </c>
       <c r="F18">
-        <f t="shared" si="2"/>
-        <v>4.34</v>
+        <f>B18-A$5</f>
+        <v>13.479999999999999</v>
       </c>
       <c r="G18">
-        <f t="shared" si="3"/>
-        <v>3.5700000000000003</v>
+        <f>C18-B$5</f>
+        <v>9.66</v>
       </c>
       <c r="H18">
-        <f t="shared" si="4"/>
+        <f>D18-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="B19" s="6">
-        <v>16.79</v>
+        <v>22.88</v>
       </c>
       <c r="C19" s="6">
-        <v>7.57</v>
+        <v>16.71</v>
       </c>
       <c r="D19" s="6">
         <v>7.46</v>
       </c>
       <c r="F19">
-        <f t="shared" si="2"/>
-        <v>7.3899999999999988</v>
+        <f>B19-A$5</f>
+        <v>13.479999999999999</v>
       </c>
       <c r="G19">
-        <f t="shared" si="3"/>
-        <v>3.5700000000000003</v>
+        <f>C19-B$5</f>
+        <v>12.71</v>
       </c>
       <c r="H19">
-        <f t="shared" si="4"/>
+        <f>D19-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="B20" s="6">
-        <v>19.84</v>
+        <v>22.88</v>
       </c>
       <c r="C20" s="6">
-        <v>7.57</v>
+        <v>19.760000000000002</v>
       </c>
       <c r="D20" s="6">
         <v>7.46</v>
       </c>
       <c r="F20">
-        <f t="shared" si="2"/>
-        <v>10.44</v>
+        <f>B20-A$5</f>
+        <v>13.479999999999999</v>
       </c>
       <c r="G20">
-        <f t="shared" si="3"/>
-        <v>3.5700000000000003</v>
+        <f>C20-B$5</f>
+        <v>15.760000000000002</v>
       </c>
       <c r="H20">
-        <f t="shared" si="4"/>
+        <f>D20-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B21" s="6">
         <v>22.88</v>
       </c>
       <c r="C21" s="6">
-        <v>7.57</v>
+        <v>22.81</v>
       </c>
       <c r="D21" s="6">
         <v>7.46</v>
       </c>
       <c r="F21">
-        <f t="shared" si="2"/>
+        <f>B21-A$5</f>
         <v>13.479999999999999</v>
       </c>
       <c r="G21">
-        <f t="shared" si="3"/>
-        <v>3.5700000000000003</v>
+        <f>C21-B$5</f>
+        <v>18.809999999999999</v>
       </c>
       <c r="H21">
-        <f t="shared" si="4"/>
+        <f>D21-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B22" s="6">
-        <v>25.93</v>
+        <v>19.84</v>
       </c>
       <c r="C22" s="6">
-        <v>7.57</v>
+        <v>13.66</v>
       </c>
       <c r="D22" s="6">
         <v>7.46</v>
       </c>
       <c r="F22">
-        <f t="shared" si="2"/>
-        <v>16.53</v>
+        <f>B22-A$5</f>
+        <v>10.44</v>
       </c>
       <c r="G22">
-        <f t="shared" si="3"/>
-        <v>3.5700000000000003</v>
+        <f>C22-B$5</f>
+        <v>9.66</v>
       </c>
       <c r="H22">
-        <f t="shared" si="4"/>
+        <f>D22-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B23" s="6">
-        <v>28.98</v>
+        <v>19.84</v>
       </c>
       <c r="C23" s="6">
-        <v>7.57</v>
+        <v>16.71</v>
       </c>
       <c r="D23" s="6">
         <v>7.46</v>
       </c>
       <c r="F23">
-        <f t="shared" si="2"/>
-        <v>19.579999999999998</v>
+        <f>B23-A$5</f>
+        <v>10.44</v>
       </c>
       <c r="G23">
-        <f t="shared" si="3"/>
-        <v>3.5700000000000003</v>
+        <f>C23-B$5</f>
+        <v>12.71</v>
       </c>
       <c r="H23">
-        <f t="shared" si="4"/>
+        <f>D23-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="B24" s="6">
-        <v>10.69</v>
+        <v>19.84</v>
       </c>
       <c r="C24" s="6">
-        <v>10.62</v>
+        <v>19.760000000000002</v>
       </c>
       <c r="D24" s="6">
         <v>7.46</v>
       </c>
       <c r="F24">
-        <f t="shared" si="2"/>
-        <v>1.2899999999999991</v>
+        <f>B24-A$5</f>
+        <v>10.44</v>
       </c>
       <c r="G24">
-        <f t="shared" si="3"/>
-        <v>6.6199999999999992</v>
+        <f>C24-B$5</f>
+        <v>15.760000000000002</v>
       </c>
       <c r="H24">
-        <f t="shared" si="4"/>
+        <f>D24-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="B25" s="6">
-        <v>13.74</v>
+        <v>19.84</v>
       </c>
       <c r="C25" s="6">
-        <v>10.62</v>
+        <v>22.81</v>
       </c>
       <c r="D25" s="6">
         <v>7.46</v>
       </c>
       <c r="F25">
-        <f t="shared" si="2"/>
-        <v>4.34</v>
+        <f>B25-A$5</f>
+        <v>10.44</v>
       </c>
       <c r="G25">
-        <f t="shared" si="3"/>
-        <v>6.6199999999999992</v>
+        <f>C25-B$5</f>
+        <v>18.809999999999999</v>
       </c>
       <c r="H25">
-        <f t="shared" si="4"/>
+        <f>D25-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B26" s="6">
-        <v>16.79</v>
+        <v>28.98</v>
       </c>
       <c r="C26" s="6">
-        <v>10.62</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="D26" s="6">
         <v>7.46</v>
       </c>
       <c r="F26">
-        <f t="shared" si="2"/>
-        <v>7.3899999999999988</v>
+        <f>B26-A$5</f>
+        <v>19.579999999999998</v>
       </c>
       <c r="G26">
-        <f t="shared" si="3"/>
-        <v>6.6199999999999992</v>
+        <f>C26-B$5</f>
+        <v>0.51999999999999957</v>
       </c>
       <c r="H26">
-        <f t="shared" si="4"/>
+        <f>D26-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B27" s="6">
-        <v>19.84</v>
+        <v>28.98</v>
       </c>
       <c r="C27" s="6">
-        <v>10.62</v>
+        <v>7.57</v>
       </c>
       <c r="D27" s="6">
         <v>7.46</v>
       </c>
       <c r="F27">
-        <f t="shared" si="2"/>
-        <v>10.44</v>
+        <f>B27-A$5</f>
+        <v>19.579999999999998</v>
       </c>
       <c r="G27">
-        <f t="shared" si="3"/>
-        <v>6.6199999999999992</v>
+        <f>C27-B$5</f>
+        <v>3.5700000000000003</v>
       </c>
       <c r="H27">
-        <f t="shared" si="4"/>
+        <f>D27-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B28" s="6">
-        <v>22.88</v>
+        <v>28.98</v>
       </c>
       <c r="C28" s="6">
         <v>10.62</v>
@@ -2013,362 +2013,362 @@
         <v>7.46</v>
       </c>
       <c r="F28">
-        <f t="shared" si="2"/>
-        <v>13.479999999999999</v>
+        <f>B28-A$5</f>
+        <v>19.579999999999998</v>
       </c>
       <c r="G28">
-        <f t="shared" si="3"/>
+        <f>C28-B$5</f>
         <v>6.6199999999999992</v>
       </c>
       <c r="H28">
-        <f t="shared" si="4"/>
+        <f>D28-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B29" s="6">
         <v>25.93</v>
       </c>
       <c r="C29" s="6">
-        <v>10.62</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="D29" s="6">
         <v>7.46</v>
       </c>
       <c r="F29">
-        <f t="shared" si="2"/>
+        <f>B29-A$5</f>
         <v>16.53</v>
       </c>
       <c r="G29">
-        <f t="shared" si="3"/>
-        <v>6.6199999999999992</v>
+        <f>C29-B$5</f>
+        <v>0.51999999999999957</v>
       </c>
       <c r="H29">
-        <f t="shared" si="4"/>
+        <f>D29-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B30" s="6">
-        <v>28.98</v>
+        <v>25.93</v>
       </c>
       <c r="C30" s="6">
-        <v>10.62</v>
+        <v>7.57</v>
       </c>
       <c r="D30" s="6">
         <v>7.46</v>
       </c>
       <c r="F30">
-        <f t="shared" si="2"/>
-        <v>19.579999999999998</v>
+        <f>B30-A$5</f>
+        <v>16.53</v>
       </c>
       <c r="G30">
-        <f t="shared" si="3"/>
-        <v>6.6199999999999992</v>
+        <f>C30-B$5</f>
+        <v>3.5700000000000003</v>
       </c>
       <c r="H30">
-        <f t="shared" si="4"/>
+        <f>D30-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="B31" s="6">
-        <v>10.69</v>
+        <v>25.93</v>
       </c>
       <c r="C31" s="6">
-        <v>13.66</v>
+        <v>10.62</v>
       </c>
       <c r="D31" s="6">
         <v>7.46</v>
       </c>
       <c r="F31">
-        <f t="shared" si="2"/>
-        <v>1.2899999999999991</v>
+        <f>B31-A$5</f>
+        <v>16.53</v>
       </c>
       <c r="G31">
-        <f t="shared" si="3"/>
-        <v>9.66</v>
+        <f>C31-B$5</f>
+        <v>6.6199999999999992</v>
       </c>
       <c r="H31">
-        <f t="shared" si="4"/>
+        <f>D31-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B32" s="6">
-        <v>13.74</v>
+        <v>22.88</v>
       </c>
       <c r="C32" s="6">
-        <v>13.66</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="D32" s="6">
         <v>7.46</v>
       </c>
       <c r="F32">
-        <f t="shared" si="2"/>
-        <v>4.34</v>
+        <f>B32-A$5</f>
+        <v>13.479999999999999</v>
       </c>
       <c r="G32">
-        <f t="shared" si="3"/>
-        <v>9.66</v>
+        <f>C32-B$5</f>
+        <v>0.51999999999999957</v>
       </c>
       <c r="H32">
-        <f t="shared" si="4"/>
+        <f>D32-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B33" s="6">
-        <v>16.79</v>
+        <v>22.88</v>
       </c>
       <c r="C33" s="6">
-        <v>13.66</v>
+        <v>7.57</v>
       </c>
       <c r="D33" s="6">
         <v>7.46</v>
       </c>
       <c r="F33">
-        <f t="shared" si="2"/>
-        <v>7.3899999999999988</v>
+        <f>B33-A$5</f>
+        <v>13.479999999999999</v>
       </c>
       <c r="G33">
-        <f t="shared" si="3"/>
-        <v>9.66</v>
+        <f>C33-B$5</f>
+        <v>3.5700000000000003</v>
       </c>
       <c r="H33">
-        <f t="shared" si="4"/>
+        <f>D33-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="B34" s="6">
-        <v>19.84</v>
+        <v>22.88</v>
       </c>
       <c r="C34" s="6">
-        <v>13.66</v>
+        <v>10.62</v>
       </c>
       <c r="D34" s="6">
         <v>7.46</v>
       </c>
       <c r="F34">
-        <f t="shared" si="2"/>
-        <v>10.44</v>
+        <f>B34-A$5</f>
+        <v>13.479999999999999</v>
       </c>
       <c r="G34">
-        <f t="shared" si="3"/>
-        <v>9.66</v>
+        <f>C34-B$5</f>
+        <v>6.6199999999999992</v>
       </c>
       <c r="H34">
-        <f t="shared" si="4"/>
+        <f>D34-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="B35" s="6">
-        <v>22.88</v>
+        <v>19.84</v>
       </c>
       <c r="C35" s="6">
-        <v>13.66</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="D35" s="6">
         <v>7.46</v>
       </c>
       <c r="F35">
-        <f t="shared" si="2"/>
-        <v>13.479999999999999</v>
+        <f>B35-A$5</f>
+        <v>10.44</v>
       </c>
       <c r="G35">
-        <f t="shared" si="3"/>
-        <v>9.66</v>
+        <f>C35-B$5</f>
+        <v>0.51999999999999957</v>
       </c>
       <c r="H35">
-        <f t="shared" si="4"/>
+        <f>D35-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="B36" s="6">
-        <v>25.93</v>
+        <v>19.84</v>
       </c>
       <c r="C36" s="6">
-        <v>13.66</v>
+        <v>7.57</v>
       </c>
       <c r="D36" s="6">
         <v>7.46</v>
       </c>
       <c r="F36">
-        <f t="shared" si="2"/>
-        <v>16.53</v>
+        <f>B36-A$5</f>
+        <v>10.44</v>
       </c>
       <c r="G36">
-        <f t="shared" si="3"/>
-        <v>9.66</v>
+        <f>C36-B$5</f>
+        <v>3.5700000000000003</v>
       </c>
       <c r="H36">
-        <f t="shared" si="4"/>
+        <f>D36-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="B37" s="6">
-        <v>28.98</v>
+        <v>19.84</v>
       </c>
       <c r="C37" s="6">
-        <v>13.66</v>
+        <v>10.62</v>
       </c>
       <c r="D37" s="6">
         <v>7.46</v>
       </c>
       <c r="F37">
-        <f t="shared" si="2"/>
-        <v>19.579999999999998</v>
+        <f>B37-A$5</f>
+        <v>10.44</v>
       </c>
       <c r="G37">
-        <f t="shared" si="3"/>
-        <v>9.66</v>
+        <f>C37-B$5</f>
+        <v>6.6199999999999992</v>
       </c>
       <c r="H37">
-        <f t="shared" si="4"/>
+        <f>D37-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B38" s="6">
-        <v>10.69</v>
+        <v>16.79</v>
       </c>
       <c r="C38" s="6">
-        <v>16.71</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="D38" s="6">
         <v>7.46</v>
       </c>
       <c r="F38">
-        <f t="shared" si="2"/>
-        <v>1.2899999999999991</v>
+        <f>B38-A$5</f>
+        <v>7.3899999999999988</v>
       </c>
       <c r="G38">
-        <f t="shared" si="3"/>
-        <v>12.71</v>
+        <f>C38-B$5</f>
+        <v>0.51999999999999957</v>
       </c>
       <c r="H38">
-        <f t="shared" si="4"/>
+        <f>D38-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B39" s="6">
-        <v>13.74</v>
+        <v>16.79</v>
       </c>
       <c r="C39" s="6">
-        <v>16.71</v>
+        <v>7.57</v>
       </c>
       <c r="D39" s="6">
         <v>7.46</v>
       </c>
       <c r="F39">
-        <f t="shared" si="2"/>
-        <v>4.34</v>
+        <f>B39-A$5</f>
+        <v>7.3899999999999988</v>
       </c>
       <c r="G39">
-        <f t="shared" si="3"/>
-        <v>12.71</v>
+        <f>C39-B$5</f>
+        <v>3.5700000000000003</v>
       </c>
       <c r="H39">
-        <f t="shared" si="4"/>
+        <f>D39-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B40" s="6">
         <v>16.79</v>
       </c>
       <c r="C40" s="6">
-        <v>16.71</v>
+        <v>10.62</v>
       </c>
       <c r="D40" s="6">
         <v>7.46</v>
       </c>
       <c r="F40">
-        <f t="shared" si="2"/>
+        <f>B40-A$5</f>
         <v>7.3899999999999988</v>
       </c>
       <c r="G40">
-        <f t="shared" si="3"/>
-        <v>12.71</v>
+        <f>C40-B$5</f>
+        <v>6.6199999999999992</v>
       </c>
       <c r="H40">
-        <f t="shared" si="4"/>
+        <f>D40-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="B41" s="6">
-        <v>19.84</v>
+        <v>16.79</v>
       </c>
       <c r="C41" s="6">
-        <v>16.71</v>
+        <v>13.66</v>
       </c>
       <c r="D41" s="6">
         <v>7.46</v>
       </c>
       <c r="F41">
-        <f t="shared" si="2"/>
-        <v>10.44</v>
+        <f>B41-A$5</f>
+        <v>7.3899999999999988</v>
       </c>
       <c r="G41">
-        <f t="shared" si="3"/>
-        <v>12.71</v>
+        <f>C41-B$5</f>
+        <v>9.66</v>
       </c>
       <c r="H41">
-        <f t="shared" si="4"/>
+        <f>D41-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="B42" s="6">
-        <v>22.88</v>
+        <v>16.79</v>
       </c>
       <c r="C42" s="6">
         <v>16.71</v>
@@ -2377,206 +2377,206 @@
         <v>7.46</v>
       </c>
       <c r="F42">
-        <f t="shared" si="2"/>
-        <v>13.479999999999999</v>
+        <f>B42-A$5</f>
+        <v>7.3899999999999988</v>
       </c>
       <c r="G42">
-        <f t="shared" si="3"/>
+        <f>C42-B$5</f>
         <v>12.71</v>
       </c>
       <c r="H42">
-        <f t="shared" si="4"/>
+        <f>D42-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="B43" s="6">
-        <v>25.93</v>
+        <v>16.79</v>
       </c>
       <c r="C43" s="6">
-        <v>16.71</v>
+        <v>19.760000000000002</v>
       </c>
       <c r="D43" s="6">
         <v>7.46</v>
       </c>
       <c r="F43">
-        <f t="shared" si="2"/>
-        <v>16.53</v>
+        <f>B43-A$5</f>
+        <v>7.3899999999999988</v>
       </c>
       <c r="G43">
-        <f t="shared" si="3"/>
-        <v>12.71</v>
+        <f>C43-B$5</f>
+        <v>15.760000000000002</v>
       </c>
       <c r="H43">
-        <f t="shared" si="4"/>
+        <f>D43-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="B44" s="6">
-        <v>28.98</v>
+        <v>16.79</v>
       </c>
       <c r="C44" s="6">
-        <v>16.71</v>
+        <v>22.81</v>
       </c>
       <c r="D44" s="6">
         <v>7.46</v>
       </c>
       <c r="F44">
-        <f t="shared" si="2"/>
-        <v>19.579999999999998</v>
+        <f>B44-A$5</f>
+        <v>7.3899999999999988</v>
       </c>
       <c r="G44">
-        <f t="shared" si="3"/>
-        <v>12.71</v>
+        <f>C44-B$5</f>
+        <v>18.809999999999999</v>
       </c>
       <c r="H44">
-        <f t="shared" si="4"/>
+        <f>D44-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B45" s="6">
-        <v>10.69</v>
+        <v>13.74</v>
       </c>
       <c r="C45" s="6">
-        <v>19.760000000000002</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="D45" s="6">
         <v>7.46</v>
       </c>
       <c r="F45">
-        <f t="shared" si="2"/>
-        <v>1.2899999999999991</v>
+        <f>B45-A$5</f>
+        <v>4.34</v>
       </c>
       <c r="G45">
-        <f t="shared" si="3"/>
-        <v>15.760000000000002</v>
+        <f>C45-B$5</f>
+        <v>0.51999999999999957</v>
       </c>
       <c r="H45">
-        <f t="shared" si="4"/>
+        <f>D45-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B46" s="6">
         <v>13.74</v>
       </c>
       <c r="C46" s="6">
-        <v>19.760000000000002</v>
+        <v>7.57</v>
       </c>
       <c r="D46" s="6">
         <v>7.46</v>
       </c>
       <c r="F46">
-        <f t="shared" si="2"/>
+        <f>B46-A$5</f>
         <v>4.34</v>
       </c>
       <c r="G46">
-        <f t="shared" si="3"/>
-        <v>15.760000000000002</v>
+        <f>C46-B$5</f>
+        <v>3.5700000000000003</v>
       </c>
       <c r="H46">
-        <f t="shared" si="4"/>
+        <f>D46-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B47" s="6">
-        <v>16.79</v>
+        <v>13.74</v>
       </c>
       <c r="C47" s="6">
-        <v>19.760000000000002</v>
+        <v>10.62</v>
       </c>
       <c r="D47" s="6">
         <v>7.46</v>
       </c>
       <c r="F47">
-        <f t="shared" si="2"/>
-        <v>7.3899999999999988</v>
+        <f>B47-A$5</f>
+        <v>4.34</v>
       </c>
       <c r="G47">
-        <f t="shared" si="3"/>
-        <v>15.760000000000002</v>
+        <f>C47-B$5</f>
+        <v>6.6199999999999992</v>
       </c>
       <c r="H47">
-        <f t="shared" si="4"/>
+        <f>D47-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="B48" s="6">
-        <v>19.84</v>
+        <v>13.74</v>
       </c>
       <c r="C48" s="6">
-        <v>19.760000000000002</v>
+        <v>13.66</v>
       </c>
       <c r="D48" s="6">
         <v>7.46</v>
       </c>
       <c r="F48">
-        <f t="shared" si="2"/>
-        <v>10.44</v>
+        <f>B48-A$5</f>
+        <v>4.34</v>
       </c>
       <c r="G48">
-        <f t="shared" si="3"/>
-        <v>15.760000000000002</v>
+        <f>C48-B$5</f>
+        <v>9.66</v>
       </c>
       <c r="H48">
-        <f t="shared" si="4"/>
+        <f>D48-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="B49" s="6">
-        <v>22.88</v>
+        <v>13.74</v>
       </c>
       <c r="C49" s="6">
-        <v>19.760000000000002</v>
+        <v>16.71</v>
       </c>
       <c r="D49" s="6">
         <v>7.46</v>
       </c>
       <c r="F49">
-        <f t="shared" si="2"/>
-        <v>13.479999999999999</v>
+        <f>B49-A$5</f>
+        <v>4.34</v>
       </c>
       <c r="G49">
-        <f t="shared" si="3"/>
-        <v>15.760000000000002</v>
+        <f>C49-B$5</f>
+        <v>12.71</v>
       </c>
       <c r="H49">
-        <f t="shared" si="4"/>
+        <f>D49-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="B50" s="6">
-        <v>25.93</v>
+        <v>13.74</v>
       </c>
       <c r="C50" s="6">
         <v>19.760000000000002</v>
@@ -2585,206 +2585,206 @@
         <v>7.46</v>
       </c>
       <c r="F50">
-        <f t="shared" si="2"/>
-        <v>16.53</v>
+        <f>B50-A$5</f>
+        <v>4.34</v>
       </c>
       <c r="G50">
-        <f t="shared" si="3"/>
+        <f>C50-B$5</f>
         <v>15.760000000000002</v>
       </c>
       <c r="H50">
-        <f t="shared" si="4"/>
+        <f>D50-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
-        <v>52</v>
+        <v>97</v>
       </c>
       <c r="B51" s="6">
-        <v>28.98</v>
+        <v>13.74</v>
       </c>
       <c r="C51" s="6">
-        <v>19.760000000000002</v>
+        <v>22.81</v>
       </c>
       <c r="D51" s="6">
         <v>7.46</v>
       </c>
       <c r="F51">
-        <f t="shared" si="2"/>
-        <v>19.579999999999998</v>
+        <f>B51-A$5</f>
+        <v>4.34</v>
       </c>
       <c r="G51">
-        <f t="shared" si="3"/>
-        <v>15.760000000000002</v>
+        <f>C51-B$5</f>
+        <v>18.809999999999999</v>
       </c>
       <c r="H51">
-        <f t="shared" si="4"/>
+        <f>D51-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B52" s="6">
         <v>10.69</v>
       </c>
       <c r="C52" s="6">
-        <v>22.81</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="D52" s="6">
         <v>7.46</v>
       </c>
       <c r="F52">
-        <f t="shared" si="2"/>
+        <f>B52-A$5</f>
         <v>1.2899999999999991</v>
       </c>
       <c r="G52">
-        <f t="shared" si="3"/>
-        <v>18.809999999999999</v>
+        <f>C52-B$5</f>
+        <v>0.51999999999999957</v>
       </c>
       <c r="H52">
-        <f t="shared" si="4"/>
+        <f>D52-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B53" s="6">
-        <v>13.74</v>
+        <v>10.69</v>
       </c>
       <c r="C53" s="6">
-        <v>22.81</v>
+        <v>7.57</v>
       </c>
       <c r="D53" s="6">
         <v>7.46</v>
       </c>
       <c r="F53">
-        <f t="shared" si="2"/>
-        <v>4.34</v>
+        <f>B53-A$5</f>
+        <v>1.2899999999999991</v>
       </c>
       <c r="G53">
-        <f t="shared" si="3"/>
-        <v>18.809999999999999</v>
+        <f>C53-B$5</f>
+        <v>3.5700000000000003</v>
       </c>
       <c r="H53">
-        <f t="shared" si="4"/>
+        <f>D53-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="B54" s="6">
-        <v>16.79</v>
+        <v>10.69</v>
       </c>
       <c r="C54" s="6">
-        <v>22.81</v>
+        <v>10.62</v>
       </c>
       <c r="D54" s="6">
         <v>7.46</v>
       </c>
       <c r="F54">
-        <f t="shared" si="2"/>
-        <v>7.3899999999999988</v>
+        <f>B54-A$5</f>
+        <v>1.2899999999999991</v>
       </c>
       <c r="G54">
-        <f t="shared" si="3"/>
-        <v>18.809999999999999</v>
+        <f>C54-B$5</f>
+        <v>6.6199999999999992</v>
       </c>
       <c r="H54">
-        <f t="shared" si="4"/>
+        <f>D54-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="B55" s="6">
-        <v>19.84</v>
+        <v>10.69</v>
       </c>
       <c r="C55" s="6">
-        <v>22.81</v>
+        <v>13.66</v>
       </c>
       <c r="D55" s="6">
         <v>7.46</v>
       </c>
       <c r="F55">
-        <f t="shared" si="2"/>
-        <v>10.44</v>
+        <f>B55-A$5</f>
+        <v>1.2899999999999991</v>
       </c>
       <c r="G55">
-        <f t="shared" si="3"/>
-        <v>18.809999999999999</v>
+        <f>C55-B$5</f>
+        <v>9.66</v>
       </c>
       <c r="H55">
-        <f t="shared" si="4"/>
+        <f>D55-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="B56" s="6">
-        <v>22.88</v>
+        <v>10.69</v>
       </c>
       <c r="C56" s="6">
-        <v>22.81</v>
+        <v>16.71</v>
       </c>
       <c r="D56" s="6">
         <v>7.46</v>
       </c>
       <c r="F56">
-        <f t="shared" si="2"/>
-        <v>13.479999999999999</v>
+        <f>B56-A$5</f>
+        <v>1.2899999999999991</v>
       </c>
       <c r="G56">
-        <f t="shared" si="3"/>
-        <v>18.809999999999999</v>
+        <f>C56-B$5</f>
+        <v>12.71</v>
       </c>
       <c r="H56">
-        <f t="shared" si="4"/>
+        <f>D56-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="B57" s="6">
-        <v>25.93</v>
+        <v>10.69</v>
       </c>
       <c r="C57" s="6">
-        <v>22.81</v>
+        <v>19.760000000000002</v>
       </c>
       <c r="D57" s="6">
         <v>7.46</v>
       </c>
       <c r="F57">
-        <f t="shared" si="2"/>
-        <v>16.53</v>
+        <f>B57-A$5</f>
+        <v>1.2899999999999991</v>
       </c>
       <c r="G57">
-        <f t="shared" si="3"/>
-        <v>18.809999999999999</v>
+        <f>C57-B$5</f>
+        <v>15.760000000000002</v>
       </c>
       <c r="H57">
-        <f t="shared" si="4"/>
+        <f>D57-C$5</f>
         <v>7.46</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="B58" s="6">
-        <v>28.98</v>
+        <v>10.69</v>
       </c>
       <c r="C58" s="6">
         <v>22.81</v>
@@ -2793,15 +2793,15 @@
         <v>7.46</v>
       </c>
       <c r="F58">
-        <f t="shared" si="2"/>
-        <v>19.579999999999998</v>
+        <f>B58-A$5</f>
+        <v>1.2899999999999991</v>
       </c>
       <c r="G58">
-        <f t="shared" si="3"/>
+        <f>C58-B$5</f>
         <v>18.809999999999999</v>
       </c>
       <c r="H58">
-        <f t="shared" si="4"/>
+        <f>D58-C$5</f>
         <v>7.46</v>
       </c>
     </row>
@@ -2825,14 +2825,14 @@
       </c>
       <c r="E62">
         <f>F10</f>
-        <v>1.2899999999999991</v>
+        <v>19.579999999999998</v>
       </c>
       <c r="F62">
-        <f t="shared" ref="F62:G62" si="5">G10</f>
-        <v>0.51999999999999957</v>
+        <f>G10</f>
+        <v>9.66</v>
       </c>
       <c r="G62">
-        <f t="shared" si="5"/>
+        <f>H10</f>
         <v>7.46</v>
       </c>
       <c r="H62">
@@ -2846,7 +2846,7 @@
       </c>
       <c r="K62" s="7">
         <f>A10</f>
-        <v>98</v>
+        <v>50</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -2863,15 +2863,15 @@
         <v>347.15</v>
       </c>
       <c r="E63">
-        <f t="shared" ref="E63:G63" si="6">F11</f>
-        <v>4.34</v>
+        <f>F11</f>
+        <v>19.579999999999998</v>
       </c>
       <c r="F63">
-        <f t="shared" si="6"/>
-        <v>0.51999999999999957</v>
+        <f>G11</f>
+        <v>12.71</v>
       </c>
       <c r="G63">
-        <f t="shared" si="6"/>
+        <f>H11</f>
         <v>7.46</v>
       </c>
       <c r="H63">
@@ -2884,8 +2884,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K63" s="7">
-        <f t="shared" ref="K63:K110" si="7">A11</f>
-        <v>91</v>
+        <f>A11</f>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -2902,15 +2902,15 @@
         <v>347.15</v>
       </c>
       <c r="E64">
-        <f t="shared" ref="E64:G64" si="8">F12</f>
-        <v>7.3899999999999988</v>
+        <f>F12</f>
+        <v>19.579999999999998</v>
       </c>
       <c r="F64">
-        <f t="shared" si="8"/>
-        <v>0.51999999999999957</v>
+        <f>G12</f>
+        <v>15.760000000000002</v>
       </c>
       <c r="G64">
-        <f t="shared" si="8"/>
+        <f>H12</f>
         <v>7.46</v>
       </c>
       <c r="H64">
@@ -2923,8 +2923,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K64" s="7">
-        <f t="shared" si="7"/>
-        <v>84</v>
+        <f>A12</f>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -2941,15 +2941,15 @@
         <v>347.15</v>
       </c>
       <c r="E65">
-        <f t="shared" ref="E65:G65" si="9">F13</f>
-        <v>10.44</v>
+        <f>F13</f>
+        <v>19.579999999999998</v>
       </c>
       <c r="F65">
-        <f t="shared" si="9"/>
-        <v>0.51999999999999957</v>
+        <f>G13</f>
+        <v>18.809999999999999</v>
       </c>
       <c r="G65">
-        <f t="shared" si="9"/>
+        <f>H13</f>
         <v>7.46</v>
       </c>
       <c r="H65">
@@ -2962,8 +2962,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K65" s="7">
-        <f t="shared" si="7"/>
-        <v>81</v>
+        <f>A13</f>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -2980,15 +2980,15 @@
         <v>347.15</v>
       </c>
       <c r="E66">
-        <f t="shared" ref="E66:G66" si="10">F14</f>
-        <v>13.479999999999999</v>
+        <f>F14</f>
+        <v>16.53</v>
       </c>
       <c r="F66">
-        <f t="shared" si="10"/>
-        <v>0.51999999999999957</v>
+        <f>G14</f>
+        <v>9.66</v>
       </c>
       <c r="G66">
-        <f t="shared" si="10"/>
+        <f>H14</f>
         <v>7.46</v>
       </c>
       <c r="H66">
@@ -3001,8 +3001,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K66" s="7">
-        <f t="shared" si="7"/>
-        <v>78</v>
+        <f>A14</f>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -3019,15 +3019,15 @@
         <v>347.15</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:G67" si="11">F15</f>
+        <f>F15</f>
         <v>16.53</v>
       </c>
       <c r="F67">
-        <f t="shared" si="11"/>
-        <v>0.51999999999999957</v>
+        <f>G15</f>
+        <v>12.71</v>
       </c>
       <c r="G67">
-        <f t="shared" si="11"/>
+        <f>H15</f>
         <v>7.46</v>
       </c>
       <c r="H67">
@@ -3040,8 +3040,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K67" s="7">
-        <f t="shared" si="7"/>
-        <v>75</v>
+        <f>A15</f>
+        <v>55</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -3058,15 +3058,15 @@
         <v>347.15</v>
       </c>
       <c r="E68">
-        <f t="shared" ref="E68:G68" si="12">F16</f>
-        <v>19.579999999999998</v>
+        <f>F16</f>
+        <v>16.53</v>
       </c>
       <c r="F68">
-        <f t="shared" si="12"/>
-        <v>0.51999999999999957</v>
+        <f>G16</f>
+        <v>15.760000000000002</v>
       </c>
       <c r="G68">
-        <f t="shared" si="12"/>
+        <f>H16</f>
         <v>7.46</v>
       </c>
       <c r="H68">
@@ -3079,8 +3079,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K68" s="7">
-        <f t="shared" si="7"/>
-        <v>72</v>
+        <f>A16</f>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -3097,15 +3097,15 @@
         <v>347.15</v>
       </c>
       <c r="E69">
-        <f t="shared" ref="E69:G69" si="13">F17</f>
-        <v>1.2899999999999991</v>
+        <f>F17</f>
+        <v>16.53</v>
       </c>
       <c r="F69">
-        <f t="shared" si="13"/>
-        <v>3.5700000000000003</v>
+        <f>G17</f>
+        <v>18.809999999999999</v>
       </c>
       <c r="G69">
-        <f t="shared" si="13"/>
+        <f>H17</f>
         <v>7.46</v>
       </c>
       <c r="H69">
@@ -3118,8 +3118,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K69" s="7">
-        <f t="shared" si="7"/>
-        <v>99</v>
+        <f>A17</f>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -3136,15 +3136,15 @@
         <v>347.15</v>
       </c>
       <c r="E70">
-        <f t="shared" ref="E70:G70" si="14">F18</f>
-        <v>4.34</v>
+        <f>F18</f>
+        <v>13.479999999999999</v>
       </c>
       <c r="F70">
-        <f t="shared" si="14"/>
-        <v>3.5700000000000003</v>
+        <f>G18</f>
+        <v>9.66</v>
       </c>
       <c r="G70">
-        <f t="shared" si="14"/>
+        <f>H18</f>
         <v>7.46</v>
       </c>
       <c r="H70">
@@ -3157,8 +3157,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K70" s="7">
-        <f t="shared" si="7"/>
-        <v>92</v>
+        <f>A18</f>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -3175,15 +3175,15 @@
         <v>347.15</v>
       </c>
       <c r="E71">
-        <f t="shared" ref="E71:G71" si="15">F19</f>
-        <v>7.3899999999999988</v>
+        <f>F19</f>
+        <v>13.479999999999999</v>
       </c>
       <c r="F71">
-        <f t="shared" si="15"/>
-        <v>3.5700000000000003</v>
+        <f>G19</f>
+        <v>12.71</v>
       </c>
       <c r="G71">
-        <f t="shared" si="15"/>
+        <f>H19</f>
         <v>7.46</v>
       </c>
       <c r="H71">
@@ -3196,8 +3196,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K71" s="7">
-        <f t="shared" si="7"/>
-        <v>85</v>
+        <f>A19</f>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -3214,15 +3214,15 @@
         <v>347.15</v>
       </c>
       <c r="E72">
-        <f t="shared" ref="E72:G72" si="16">F20</f>
-        <v>10.44</v>
+        <f>F20</f>
+        <v>13.479999999999999</v>
       </c>
       <c r="F72">
-        <f t="shared" si="16"/>
-        <v>3.5700000000000003</v>
+        <f>G20</f>
+        <v>15.760000000000002</v>
       </c>
       <c r="G72">
-        <f t="shared" si="16"/>
+        <f>H20</f>
         <v>7.46</v>
       </c>
       <c r="H72">
@@ -3235,8 +3235,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K72" s="7">
-        <f t="shared" si="7"/>
-        <v>82</v>
+        <f>A20</f>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -3253,15 +3253,15 @@
         <v>347.15</v>
       </c>
       <c r="E73">
-        <f t="shared" ref="E73:G73" si="17">F21</f>
+        <f>F21</f>
         <v>13.479999999999999</v>
       </c>
       <c r="F73">
-        <f t="shared" si="17"/>
-        <v>3.5700000000000003</v>
+        <f>G21</f>
+        <v>18.809999999999999</v>
       </c>
       <c r="G73">
-        <f t="shared" si="17"/>
+        <f>H21</f>
         <v>7.46</v>
       </c>
       <c r="H73">
@@ -3274,8 +3274,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K73" s="7">
-        <f t="shared" si="7"/>
-        <v>79</v>
+        <f>A21</f>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -3292,15 +3292,15 @@
         <v>347.15</v>
       </c>
       <c r="E74">
-        <f t="shared" ref="E74:G74" si="18">F22</f>
-        <v>16.53</v>
+        <f>F22</f>
+        <v>10.44</v>
       </c>
       <c r="F74">
-        <f t="shared" si="18"/>
-        <v>3.5700000000000003</v>
+        <f>G22</f>
+        <v>9.66</v>
       </c>
       <c r="G74">
-        <f t="shared" si="18"/>
+        <f>H22</f>
         <v>7.46</v>
       </c>
       <c r="H74">
@@ -3313,8 +3313,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K74" s="7">
-        <f t="shared" si="7"/>
-        <v>76</v>
+        <f>A22</f>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -3331,15 +3331,15 @@
         <v>347.15</v>
       </c>
       <c r="E75">
-        <f t="shared" ref="E75:G75" si="19">F23</f>
-        <v>19.579999999999998</v>
+        <f>F23</f>
+        <v>10.44</v>
       </c>
       <c r="F75">
-        <f t="shared" si="19"/>
-        <v>3.5700000000000003</v>
+        <f>G23</f>
+        <v>12.71</v>
       </c>
       <c r="G75">
-        <f t="shared" si="19"/>
+        <f>H23</f>
         <v>7.46</v>
       </c>
       <c r="H75">
@@ -3352,8 +3352,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K75" s="7">
-        <f t="shared" si="7"/>
-        <v>73</v>
+        <f>A23</f>
+        <v>63</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
@@ -3370,15 +3370,15 @@
         <v>347.15</v>
       </c>
       <c r="E76">
-        <f t="shared" ref="E76:G76" si="20">F24</f>
-        <v>1.2899999999999991</v>
+        <f>F24</f>
+        <v>10.44</v>
       </c>
       <c r="F76">
-        <f t="shared" si="20"/>
-        <v>6.6199999999999992</v>
+        <f>G24</f>
+        <v>15.760000000000002</v>
       </c>
       <c r="G76">
-        <f t="shared" si="20"/>
+        <f>H24</f>
         <v>7.46</v>
       </c>
       <c r="H76">
@@ -3391,8 +3391,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K76" s="7">
-        <f t="shared" si="7"/>
-        <v>100</v>
+        <f>A24</f>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -3409,15 +3409,15 @@
         <v>347.15</v>
       </c>
       <c r="E77">
-        <f t="shared" ref="E77:G77" si="21">F25</f>
-        <v>4.34</v>
+        <f>F25</f>
+        <v>10.44</v>
       </c>
       <c r="F77">
-        <f t="shared" si="21"/>
-        <v>6.6199999999999992</v>
+        <f>G25</f>
+        <v>18.809999999999999</v>
       </c>
       <c r="G77">
-        <f t="shared" si="21"/>
+        <f>H25</f>
         <v>7.46</v>
       </c>
       <c r="H77">
@@ -3430,8 +3430,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K77" s="7">
-        <f t="shared" si="7"/>
-        <v>93</v>
+        <f>A25</f>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
@@ -3448,15 +3448,15 @@
         <v>347.15</v>
       </c>
       <c r="E78">
-        <f t="shared" ref="E78:G78" si="22">F26</f>
-        <v>7.3899999999999988</v>
+        <f>F26</f>
+        <v>19.579999999999998</v>
       </c>
       <c r="F78">
-        <f t="shared" si="22"/>
-        <v>6.6199999999999992</v>
+        <f>G26</f>
+        <v>0.51999999999999957</v>
       </c>
       <c r="G78">
-        <f t="shared" si="22"/>
+        <f>H26</f>
         <v>7.46</v>
       </c>
       <c r="H78">
@@ -3469,8 +3469,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K78" s="7">
-        <f t="shared" si="7"/>
-        <v>86</v>
+        <f>A26</f>
+        <v>72</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -3487,15 +3487,15 @@
         <v>347.15</v>
       </c>
       <c r="E79">
-        <f t="shared" ref="E79:G79" si="23">F27</f>
-        <v>10.44</v>
+        <f>F27</f>
+        <v>19.579999999999998</v>
       </c>
       <c r="F79">
-        <f t="shared" si="23"/>
-        <v>6.6199999999999992</v>
+        <f>G27</f>
+        <v>3.5700000000000003</v>
       </c>
       <c r="G79">
-        <f t="shared" si="23"/>
+        <f>H27</f>
         <v>7.46</v>
       </c>
       <c r="H79">
@@ -3508,8 +3508,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K79" s="7">
-        <f t="shared" si="7"/>
-        <v>83</v>
+        <f>A27</f>
+        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
@@ -3526,15 +3526,15 @@
         <v>347.15</v>
       </c>
       <c r="E80">
-        <f t="shared" ref="E80:G80" si="24">F28</f>
-        <v>13.479999999999999</v>
+        <f>F28</f>
+        <v>19.579999999999998</v>
       </c>
       <c r="F80">
-        <f t="shared" si="24"/>
+        <f>G28</f>
         <v>6.6199999999999992</v>
       </c>
       <c r="G80">
-        <f t="shared" si="24"/>
+        <f>H28</f>
         <v>7.46</v>
       </c>
       <c r="H80">
@@ -3547,8 +3547,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K80" s="7">
-        <f t="shared" si="7"/>
-        <v>80</v>
+        <f>A28</f>
+        <v>74</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
@@ -3565,15 +3565,15 @@
         <v>347.15</v>
       </c>
       <c r="E81">
-        <f t="shared" ref="E81:G81" si="25">F29</f>
+        <f>F29</f>
         <v>16.53</v>
       </c>
       <c r="F81">
-        <f t="shared" si="25"/>
-        <v>6.6199999999999992</v>
+        <f>G29</f>
+        <v>0.51999999999999957</v>
       </c>
       <c r="G81">
-        <f t="shared" si="25"/>
+        <f>H29</f>
         <v>7.46</v>
       </c>
       <c r="H81">
@@ -3586,8 +3586,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K81" s="7">
-        <f t="shared" si="7"/>
-        <v>77</v>
+        <f>A29</f>
+        <v>75</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -3604,15 +3604,15 @@
         <v>347.15</v>
       </c>
       <c r="E82">
-        <f t="shared" ref="E82:G82" si="26">F30</f>
-        <v>19.579999999999998</v>
+        <f>F30</f>
+        <v>16.53</v>
       </c>
       <c r="F82">
-        <f t="shared" si="26"/>
-        <v>6.6199999999999992</v>
+        <f>G30</f>
+        <v>3.5700000000000003</v>
       </c>
       <c r="G82">
-        <f t="shared" si="26"/>
+        <f>H30</f>
         <v>7.46</v>
       </c>
       <c r="H82">
@@ -3625,8 +3625,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K82" s="7">
-        <f t="shared" si="7"/>
-        <v>74</v>
+        <f>A30</f>
+        <v>76</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -3643,15 +3643,15 @@
         <v>347.15</v>
       </c>
       <c r="E83">
-        <f t="shared" ref="E83:G83" si="27">F31</f>
-        <v>1.2899999999999991</v>
+        <f>F31</f>
+        <v>16.53</v>
       </c>
       <c r="F83">
-        <f t="shared" si="27"/>
-        <v>9.66</v>
+        <f>G31</f>
+        <v>6.6199999999999992</v>
       </c>
       <c r="G83">
-        <f t="shared" si="27"/>
+        <f>H31</f>
         <v>7.46</v>
       </c>
       <c r="H83">
@@ -3664,8 +3664,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K83" s="7">
-        <f t="shared" si="7"/>
-        <v>101</v>
+        <f>A31</f>
+        <v>77</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -3682,15 +3682,15 @@
         <v>347.15</v>
       </c>
       <c r="E84">
-        <f t="shared" ref="E84:G84" si="28">F32</f>
-        <v>4.34</v>
+        <f>F32</f>
+        <v>13.479999999999999</v>
       </c>
       <c r="F84">
-        <f t="shared" si="28"/>
-        <v>9.66</v>
+        <f>G32</f>
+        <v>0.51999999999999957</v>
       </c>
       <c r="G84">
-        <f t="shared" si="28"/>
+        <f>H32</f>
         <v>7.46</v>
       </c>
       <c r="H84">
@@ -3703,8 +3703,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K84" s="7">
-        <f t="shared" si="7"/>
-        <v>94</v>
+        <f>A32</f>
+        <v>78</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -3721,15 +3721,15 @@
         <v>347.15</v>
       </c>
       <c r="E85">
-        <f t="shared" ref="E85:G85" si="29">F33</f>
-        <v>7.3899999999999988</v>
+        <f>F33</f>
+        <v>13.479999999999999</v>
       </c>
       <c r="F85">
-        <f t="shared" si="29"/>
-        <v>9.66</v>
+        <f>G33</f>
+        <v>3.5700000000000003</v>
       </c>
       <c r="G85">
-        <f t="shared" si="29"/>
+        <f>H33</f>
         <v>7.46</v>
       </c>
       <c r="H85">
@@ -3742,8 +3742,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K85" s="7">
-        <f t="shared" si="7"/>
-        <v>87</v>
+        <f>A33</f>
+        <v>79</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -3760,15 +3760,15 @@
         <v>347.15</v>
       </c>
       <c r="E86">
-        <f t="shared" ref="E86:G86" si="30">F34</f>
-        <v>10.44</v>
+        <f>F34</f>
+        <v>13.479999999999999</v>
       </c>
       <c r="F86">
-        <f t="shared" si="30"/>
-        <v>9.66</v>
+        <f>G34</f>
+        <v>6.6199999999999992</v>
       </c>
       <c r="G86">
-        <f t="shared" si="30"/>
+        <f>H34</f>
         <v>7.46</v>
       </c>
       <c r="H86">
@@ -3781,8 +3781,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K86" s="7">
-        <f t="shared" si="7"/>
-        <v>62</v>
+        <f>A34</f>
+        <v>80</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
@@ -3799,15 +3799,15 @@
         <v>347.15</v>
       </c>
       <c r="E87">
-        <f t="shared" ref="E87:G87" si="31">F35</f>
-        <v>13.479999999999999</v>
+        <f>F35</f>
+        <v>10.44</v>
       </c>
       <c r="F87">
-        <f t="shared" si="31"/>
-        <v>9.66</v>
+        <f>G35</f>
+        <v>0.51999999999999957</v>
       </c>
       <c r="G87">
-        <f t="shared" si="31"/>
+        <f>H35</f>
         <v>7.46</v>
       </c>
       <c r="H87">
@@ -3820,8 +3820,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K87" s="7">
-        <f t="shared" si="7"/>
-        <v>58</v>
+        <f>A35</f>
+        <v>81</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
@@ -3838,15 +3838,15 @@
         <v>347.15</v>
       </c>
       <c r="E88">
-        <f t="shared" ref="E88:G88" si="32">F36</f>
-        <v>16.53</v>
+        <f>F36</f>
+        <v>10.44</v>
       </c>
       <c r="F88">
-        <f t="shared" si="32"/>
-        <v>9.66</v>
+        <f>G36</f>
+        <v>3.5700000000000003</v>
       </c>
       <c r="G88">
-        <f t="shared" si="32"/>
+        <f>H36</f>
         <v>7.46</v>
       </c>
       <c r="H88">
@@ -3859,8 +3859,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K88" s="7">
-        <f t="shared" si="7"/>
-        <v>54</v>
+        <f>A36</f>
+        <v>82</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
@@ -3877,15 +3877,15 @@
         <v>347.15</v>
       </c>
       <c r="E89">
-        <f t="shared" ref="E89:G89" si="33">F37</f>
-        <v>19.579999999999998</v>
+        <f>F37</f>
+        <v>10.44</v>
       </c>
       <c r="F89">
-        <f t="shared" si="33"/>
-        <v>9.66</v>
+        <f>G37</f>
+        <v>6.6199999999999992</v>
       </c>
       <c r="G89">
-        <f t="shared" si="33"/>
+        <f>H37</f>
         <v>7.46</v>
       </c>
       <c r="H89">
@@ -3898,8 +3898,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K89" s="7">
-        <f t="shared" si="7"/>
-        <v>50</v>
+        <f>A37</f>
+        <v>83</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
@@ -3916,15 +3916,15 @@
         <v>347.15</v>
       </c>
       <c r="E90">
-        <f t="shared" ref="E90:G90" si="34">F38</f>
-        <v>1.2899999999999991</v>
+        <f>F38</f>
+        <v>7.3899999999999988</v>
       </c>
       <c r="F90">
-        <f t="shared" si="34"/>
-        <v>12.71</v>
+        <f>G38</f>
+        <v>0.51999999999999957</v>
       </c>
       <c r="G90">
-        <f t="shared" si="34"/>
+        <f>H38</f>
         <v>7.46</v>
       </c>
       <c r="H90">
@@ -3937,8 +3937,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K90" s="7">
-        <f t="shared" si="7"/>
-        <v>102</v>
+        <f>A38</f>
+        <v>84</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
@@ -3955,15 +3955,15 @@
         <v>347.15</v>
       </c>
       <c r="E91">
-        <f t="shared" ref="E91:G91" si="35">F39</f>
-        <v>4.34</v>
+        <f>F39</f>
+        <v>7.3899999999999988</v>
       </c>
       <c r="F91">
-        <f t="shared" si="35"/>
-        <v>12.71</v>
+        <f>G39</f>
+        <v>3.5700000000000003</v>
       </c>
       <c r="G91">
-        <f t="shared" si="35"/>
+        <f>H39</f>
         <v>7.46</v>
       </c>
       <c r="H91">
@@ -3976,8 +3976,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K91" s="7">
-        <f t="shared" si="7"/>
-        <v>95</v>
+        <f>A39</f>
+        <v>85</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
@@ -3994,15 +3994,15 @@
         <v>347.15</v>
       </c>
       <c r="E92">
-        <f t="shared" ref="E92:G92" si="36">F40</f>
+        <f>F40</f>
         <v>7.3899999999999988</v>
       </c>
       <c r="F92">
-        <f t="shared" si="36"/>
-        <v>12.71</v>
+        <f>G40</f>
+        <v>6.6199999999999992</v>
       </c>
       <c r="G92">
-        <f t="shared" si="36"/>
+        <f>H40</f>
         <v>7.46</v>
       </c>
       <c r="H92">
@@ -4015,8 +4015,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K92" s="7">
-        <f t="shared" si="7"/>
-        <v>88</v>
+        <f>A40</f>
+        <v>86</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
@@ -4033,15 +4033,15 @@
         <v>347.15</v>
       </c>
       <c r="E93">
-        <f t="shared" ref="E93:G93" si="37">F41</f>
-        <v>10.44</v>
+        <f>F41</f>
+        <v>7.3899999999999988</v>
       </c>
       <c r="F93">
-        <f t="shared" si="37"/>
-        <v>12.71</v>
+        <f>G41</f>
+        <v>9.66</v>
       </c>
       <c r="G93">
-        <f t="shared" si="37"/>
+        <f>H41</f>
         <v>7.46</v>
       </c>
       <c r="H93">
@@ -4054,8 +4054,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K93" s="7">
-        <f t="shared" si="7"/>
-        <v>63</v>
+        <f>A41</f>
+        <v>87</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
@@ -4072,15 +4072,15 @@
         <v>347.15</v>
       </c>
       <c r="E94">
-        <f t="shared" ref="E94:G94" si="38">F42</f>
-        <v>13.479999999999999</v>
+        <f>F42</f>
+        <v>7.3899999999999988</v>
       </c>
       <c r="F94">
-        <f t="shared" si="38"/>
+        <f>G42</f>
         <v>12.71</v>
       </c>
       <c r="G94">
-        <f t="shared" si="38"/>
+        <f>H42</f>
         <v>7.46</v>
       </c>
       <c r="H94">
@@ -4093,8 +4093,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K94" s="7">
-        <f t="shared" si="7"/>
-        <v>59</v>
+        <f>A42</f>
+        <v>88</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
@@ -4111,15 +4111,15 @@
         <v>347.15</v>
       </c>
       <c r="E95">
-        <f t="shared" ref="E95:G95" si="39">F43</f>
-        <v>16.53</v>
+        <f>F43</f>
+        <v>7.3899999999999988</v>
       </c>
       <c r="F95">
-        <f t="shared" si="39"/>
-        <v>12.71</v>
+        <f>G43</f>
+        <v>15.760000000000002</v>
       </c>
       <c r="G95">
-        <f t="shared" si="39"/>
+        <f>H43</f>
         <v>7.46</v>
       </c>
       <c r="H95">
@@ -4132,8 +4132,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K95" s="7">
-        <f t="shared" si="7"/>
-        <v>55</v>
+        <f>A43</f>
+        <v>89</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
@@ -4150,15 +4150,15 @@
         <v>347.15</v>
       </c>
       <c r="E96">
-        <f t="shared" ref="E96:G96" si="40">F44</f>
-        <v>19.579999999999998</v>
+        <f>F44</f>
+        <v>7.3899999999999988</v>
       </c>
       <c r="F96">
-        <f t="shared" si="40"/>
-        <v>12.71</v>
+        <f>G44</f>
+        <v>18.809999999999999</v>
       </c>
       <c r="G96">
-        <f t="shared" si="40"/>
+        <f>H44</f>
         <v>7.46</v>
       </c>
       <c r="H96">
@@ -4171,8 +4171,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K96" s="7">
-        <f t="shared" si="7"/>
-        <v>51</v>
+        <f>A44</f>
+        <v>90</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -4189,15 +4189,15 @@
         <v>347.15</v>
       </c>
       <c r="E97">
-        <f t="shared" ref="E97:G97" si="41">F45</f>
-        <v>1.2899999999999991</v>
+        <f>F45</f>
+        <v>4.34</v>
       </c>
       <c r="F97">
-        <f t="shared" si="41"/>
-        <v>15.760000000000002</v>
+        <f>G45</f>
+        <v>0.51999999999999957</v>
       </c>
       <c r="G97">
-        <f t="shared" si="41"/>
+        <f>H45</f>
         <v>7.46</v>
       </c>
       <c r="H97">
@@ -4210,8 +4210,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K97" s="7">
-        <f t="shared" si="7"/>
-        <v>103</v>
+        <f>A45</f>
+        <v>91</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
@@ -4228,15 +4228,15 @@
         <v>347.15</v>
       </c>
       <c r="E98">
-        <f t="shared" ref="E98:G98" si="42">F46</f>
+        <f>F46</f>
         <v>4.34</v>
       </c>
       <c r="F98">
-        <f t="shared" si="42"/>
-        <v>15.760000000000002</v>
+        <f>G46</f>
+        <v>3.5700000000000003</v>
       </c>
       <c r="G98">
-        <f t="shared" si="42"/>
+        <f>H46</f>
         <v>7.46</v>
       </c>
       <c r="H98">
@@ -4249,8 +4249,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K98" s="7">
-        <f t="shared" si="7"/>
-        <v>96</v>
+        <f>A46</f>
+        <v>92</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -4267,15 +4267,15 @@
         <v>347.15</v>
       </c>
       <c r="E99">
-        <f t="shared" ref="E99:G99" si="43">F47</f>
-        <v>7.3899999999999988</v>
+        <f>F47</f>
+        <v>4.34</v>
       </c>
       <c r="F99">
-        <f t="shared" si="43"/>
-        <v>15.760000000000002</v>
+        <f>G47</f>
+        <v>6.6199999999999992</v>
       </c>
       <c r="G99">
-        <f t="shared" si="43"/>
+        <f>H47</f>
         <v>7.46</v>
       </c>
       <c r="H99">
@@ -4288,8 +4288,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K99" s="7">
-        <f t="shared" si="7"/>
-        <v>89</v>
+        <f>A47</f>
+        <v>93</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -4306,15 +4306,15 @@
         <v>347.15</v>
       </c>
       <c r="E100">
-        <f t="shared" ref="E100:G100" si="44">F48</f>
-        <v>10.44</v>
+        <f>F48</f>
+        <v>4.34</v>
       </c>
       <c r="F100">
-        <f t="shared" si="44"/>
-        <v>15.760000000000002</v>
+        <f>G48</f>
+        <v>9.66</v>
       </c>
       <c r="G100">
-        <f t="shared" si="44"/>
+        <f>H48</f>
         <v>7.46</v>
       </c>
       <c r="H100">
@@ -4327,8 +4327,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K100" s="7">
-        <f t="shared" si="7"/>
-        <v>64</v>
+        <f>A48</f>
+        <v>94</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
@@ -4345,15 +4345,15 @@
         <v>347.15</v>
       </c>
       <c r="E101">
-        <f t="shared" ref="E101:G101" si="45">F49</f>
-        <v>13.479999999999999</v>
+        <f>F49</f>
+        <v>4.34</v>
       </c>
       <c r="F101">
-        <f t="shared" si="45"/>
-        <v>15.760000000000002</v>
+        <f>G49</f>
+        <v>12.71</v>
       </c>
       <c r="G101">
-        <f t="shared" si="45"/>
+        <f>H49</f>
         <v>7.46</v>
       </c>
       <c r="H101">
@@ -4366,8 +4366,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K101" s="7">
-        <f t="shared" si="7"/>
-        <v>60</v>
+        <f>A49</f>
+        <v>95</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -4384,15 +4384,15 @@
         <v>347.15</v>
       </c>
       <c r="E102">
-        <f t="shared" ref="E102:G102" si="46">F50</f>
-        <v>16.53</v>
+        <f>F50</f>
+        <v>4.34</v>
       </c>
       <c r="F102">
-        <f t="shared" si="46"/>
+        <f>G50</f>
         <v>15.760000000000002</v>
       </c>
       <c r="G102">
-        <f t="shared" si="46"/>
+        <f>H50</f>
         <v>7.46</v>
       </c>
       <c r="H102">
@@ -4405,8 +4405,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K102" s="7">
-        <f t="shared" si="7"/>
-        <v>56</v>
+        <f>A50</f>
+        <v>96</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
@@ -4423,15 +4423,15 @@
         <v>347.15</v>
       </c>
       <c r="E103">
-        <f t="shared" ref="E103:G103" si="47">F51</f>
-        <v>19.579999999999998</v>
+        <f>F51</f>
+        <v>4.34</v>
       </c>
       <c r="F103">
-        <f t="shared" si="47"/>
-        <v>15.760000000000002</v>
+        <f>G51</f>
+        <v>18.809999999999999</v>
       </c>
       <c r="G103">
-        <f t="shared" si="47"/>
+        <f>H51</f>
         <v>7.46</v>
       </c>
       <c r="H103">
@@ -4444,8 +4444,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K103" s="7">
-        <f t="shared" si="7"/>
-        <v>52</v>
+        <f>A51</f>
+        <v>97</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
@@ -4462,15 +4462,15 @@
         <v>347.15</v>
       </c>
       <c r="E104">
-        <f t="shared" ref="E104:G104" si="48">F52</f>
+        <f>F52</f>
         <v>1.2899999999999991</v>
       </c>
       <c r="F104">
-        <f t="shared" si="48"/>
-        <v>18.809999999999999</v>
+        <f>G52</f>
+        <v>0.51999999999999957</v>
       </c>
       <c r="G104">
-        <f t="shared" si="48"/>
+        <f>H52</f>
         <v>7.46</v>
       </c>
       <c r="H104">
@@ -4483,8 +4483,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K104" s="7">
-        <f t="shared" si="7"/>
-        <v>104</v>
+        <f>A52</f>
+        <v>98</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
@@ -4501,15 +4501,15 @@
         <v>347.15</v>
       </c>
       <c r="E105">
-        <f t="shared" ref="E105:G105" si="49">F53</f>
-        <v>4.34</v>
+        <f>F53</f>
+        <v>1.2899999999999991</v>
       </c>
       <c r="F105">
-        <f t="shared" si="49"/>
-        <v>18.809999999999999</v>
+        <f>G53</f>
+        <v>3.5700000000000003</v>
       </c>
       <c r="G105">
-        <f t="shared" si="49"/>
+        <f>H53</f>
         <v>7.46</v>
       </c>
       <c r="H105">
@@ -4522,8 +4522,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K105" s="7">
-        <f t="shared" si="7"/>
-        <v>97</v>
+        <f>A53</f>
+        <v>99</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
@@ -4540,15 +4540,15 @@
         <v>347.15</v>
       </c>
       <c r="E106">
-        <f t="shared" ref="E106:G106" si="50">F54</f>
-        <v>7.3899999999999988</v>
+        <f>F54</f>
+        <v>1.2899999999999991</v>
       </c>
       <c r="F106">
-        <f t="shared" si="50"/>
-        <v>18.809999999999999</v>
+        <f>G54</f>
+        <v>6.6199999999999992</v>
       </c>
       <c r="G106">
-        <f t="shared" si="50"/>
+        <f>H54</f>
         <v>7.46</v>
       </c>
       <c r="H106">
@@ -4561,8 +4561,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K106" s="7">
-        <f t="shared" si="7"/>
-        <v>90</v>
+        <f>A54</f>
+        <v>100</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
@@ -4579,15 +4579,15 @@
         <v>347.15</v>
       </c>
       <c r="E107">
-        <f t="shared" ref="E107:G107" si="51">F55</f>
-        <v>10.44</v>
+        <f>F55</f>
+        <v>1.2899999999999991</v>
       </c>
       <c r="F107">
-        <f t="shared" si="51"/>
-        <v>18.809999999999999</v>
+        <f>G55</f>
+        <v>9.66</v>
       </c>
       <c r="G107">
-        <f t="shared" si="51"/>
+        <f>H55</f>
         <v>7.46</v>
       </c>
       <c r="H107">
@@ -4600,8 +4600,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K107" s="7">
-        <f t="shared" si="7"/>
-        <v>65</v>
+        <f>A55</f>
+        <v>101</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
@@ -4618,15 +4618,15 @@
         <v>347.15</v>
       </c>
       <c r="E108">
-        <f t="shared" ref="E108:G108" si="52">F56</f>
-        <v>13.479999999999999</v>
+        <f>F56</f>
+        <v>1.2899999999999991</v>
       </c>
       <c r="F108">
-        <f t="shared" si="52"/>
-        <v>18.809999999999999</v>
+        <f>G56</f>
+        <v>12.71</v>
       </c>
       <c r="G108">
-        <f t="shared" si="52"/>
+        <f>H56</f>
         <v>7.46</v>
       </c>
       <c r="H108">
@@ -4639,8 +4639,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K108" s="7">
-        <f t="shared" si="7"/>
-        <v>61</v>
+        <f>A56</f>
+        <v>102</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
@@ -4657,15 +4657,15 @@
         <v>347.15</v>
       </c>
       <c r="E109">
-        <f t="shared" ref="E109:G109" si="53">F57</f>
-        <v>16.53</v>
+        <f>F57</f>
+        <v>1.2899999999999991</v>
       </c>
       <c r="F109">
-        <f t="shared" si="53"/>
-        <v>18.809999999999999</v>
+        <f>G57</f>
+        <v>15.760000000000002</v>
       </c>
       <c r="G109">
-        <f t="shared" si="53"/>
+        <f>H57</f>
         <v>7.46</v>
       </c>
       <c r="H109">
@@ -4678,8 +4678,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K109" s="7">
-        <f t="shared" si="7"/>
-        <v>57</v>
+        <f>A57</f>
+        <v>103</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
@@ -4696,15 +4696,15 @@
         <v>347.15</v>
       </c>
       <c r="E110">
-        <f t="shared" ref="E110:G110" si="54">F58</f>
-        <v>19.579999999999998</v>
+        <f>F58</f>
+        <v>1.2899999999999991</v>
       </c>
       <c r="F110">
-        <f t="shared" si="54"/>
+        <f>G58</f>
         <v>18.809999999999999</v>
       </c>
       <c r="G110">
-        <f t="shared" si="54"/>
+        <f>H58</f>
         <v>7.46</v>
       </c>
       <c r="H110">
@@ -4717,8 +4717,8 @@
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="K110" s="7">
-        <f t="shared" si="7"/>
-        <v>53</v>
+        <f>A58</f>
+        <v>104</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
@@ -4898,6 +4898,9 @@
       <c r="K154" s="7"/>
     </row>
   </sheetData>
+  <sortState ref="A10:H58">
+    <sortCondition ref="A10:A58"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>